<commit_message>
chore: Migrated latest version of Doc2Rdf from dugtrio-experimental (#27)
* chore: Migrated latest version of Doc2Rdf from dugtrio-experimental

* fix: Removed RdfCommon as it was not used

* Fix: Updates based on PR feedback

Co-authored-by: bhtvedt <bhtvedt@gmail.com>
</commit_message>
<xml_diff>
--- a/Doc2Rdf/Doc2Rdf.Tests/TestData/test.xlsx
+++ b/Doc2Rdf/Doc2Rdf.Tests/TestData/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Equinor\dugtrio-experimental\Doc2Rdf\Doc2Rdf.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08C1D4C-8BFD-47E6-ACDB-80DD044F48DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B776B93-C6EC-403A-8639-4BA5D5EE687B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheetName" sheetId="1" r:id="rId1"/>
@@ -4733,9 +4733,6 @@
     <t>SheetName</t>
   </si>
   <si>
-    <t>c232</t>
-  </si>
-  <si>
     <t>RevisionDate</t>
   </si>
   <si>
@@ -4749,6 +4746,9 @@
   </si>
   <si>
     <t>Tag Number</t>
+  </si>
+  <si>
+    <t>C232</t>
   </si>
 </sst>
 </file>
@@ -5137,7 +5137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -5160,7 +5160,7 @@
         <v>1014</v>
       </c>
       <c r="E1" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="F1" t="s">
         <v>1015</v>
@@ -86648,7 +86648,7 @@
         <v>498</v>
       </c>
       <c r="BA498" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="BC498" t="s">
         <v>495</v>
@@ -86846,8 +86846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31B494F-3AF4-40F9-AC21-215D6956698A}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -86865,7 +86865,7 @@
         <v>501</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1565</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -86879,7 +86879,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1563</v>
@@ -86943,10 +86943,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B12" t="s">
         <v>1567</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>